<commit_message>
save database and api testing
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/batch14excel.xlsx
+++ b/src/test/resources/testdata/batch14excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/74d83ca33d231edf/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/74d83ca33d231edf/Desktop/IntelijProjects/CucumberBatch14/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="11_F25DC773A252ABDACC10483CD1DB58EC5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{725BDCAC-44FE-4CA3-B50E-068961875B21}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="11_F25DC773A252ABDACC10483CD1DB58EC5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FB7E65F-E4A0-44DC-AFAD-7946D60F035B}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28440" yWindow="2880" windowWidth="18000" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EmployeeData" sheetId="1" r:id="rId1"/>
@@ -51,37 +51,37 @@
     <t>ms</t>
   </si>
   <si>
-    <t>anton</t>
-  </si>
-  <si>
     <t>Syntax123!</t>
   </si>
   <si>
-    <t>iva</t>
-  </si>
-  <si>
-    <t>niko</t>
-  </si>
-  <si>
-    <t>anil</t>
-  </si>
-  <si>
-    <t>niko321</t>
-  </si>
-  <si>
-    <t>lori</t>
-  </si>
-  <si>
-    <t>hoy</t>
-  </si>
-  <si>
     <t>C:\Users\dudka\OneDrive\Desktop\picture.jpg</t>
   </si>
   <si>
-    <t>iva123</t>
-  </si>
-  <si>
-    <t>nil321</t>
+    <t>ivab</t>
+  </si>
+  <si>
+    <t>nikod</t>
+  </si>
+  <si>
+    <t>loris</t>
+  </si>
+  <si>
+    <t>antons</t>
+  </si>
+  <si>
+    <t>anilf</t>
+  </si>
+  <si>
+    <t>hoyw</t>
+  </si>
+  <si>
+    <t>ivab123</t>
+  </si>
+  <si>
+    <t>nikod321</t>
+  </si>
+  <si>
+    <t>lorisl321</t>
   </si>
 </sst>
 </file>
@@ -134,10 +134,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -449,19 +445,19 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -472,24 +468,24 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -498,16 +494,16 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
         <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>